<commit_message>
center poi / 2023.02.02 / 10:32 / sojung
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/templates/template_센터.xlsx
+++ b/src/main/webapp/resources/templates/template_센터.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KOSA\git\store-management\src\main\webapp\resources\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KOSA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D8CD81-AD2C-4051-A91B-EF355663E252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7434E5BB-A45C-4F42-9EE8-2C7D61F2A704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{59DB4302-11B8-4813-85BF-B0C8E7845784}"/>
+    <workbookView xWindow="4840" yWindow="1600" windowWidth="19200" windowHeight="11260" xr2:uid="{59DB4302-11B8-4813-85BF-B0C8E7845784}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>센터코드</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -69,6 +69,10 @@
   <si>
     <t>수정 시 기존에 등록되어 있던 센터코드는 건들지마세요</t>
     <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>전화번호, 오픈일, 폐점일은 숫자만 입력해주세요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -229,23 +233,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -649,57 +653,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4456F567-36D6-4C74-B9C9-6566919CF804}">
   <dimension ref="B2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="18.1640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="33.25" style="7" customWidth="1"/>
-    <col min="4" max="4" width="49.9140625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="45.4140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="23.4140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="16.4140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="33.25" style="6" customWidth="1"/>
+    <col min="4" max="4" width="49.9140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="45.4140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="23.4140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="16.4140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="48.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="26" x14ac:dyDescent="0.65">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="4" spans="2:11" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -717,7 +721,9 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="J7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="J8" s="2"/>
@@ -757,6 +763,24 @@
   <conditionalFormatting sqref="F6:F7">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <dataValidations count="4">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{34AACA69-3CCB-4C78-8D73-91E026CABB73}">
+      <formula1>1</formula1>
+      <formula2>20</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{7E6166F9-EB1F-4BB6-9191-006B1F8D946F}">
+      <formula1>1</formula1>
+      <formula2>7</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{9529997E-55FD-41D8-876B-00C17B2BD852}">
+      <formula1>1</formula1>
+      <formula2>50</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{1E1D24F2-1AF8-4643-918E-DEA91CF1B861}">
+      <formula1>9</formula1>
+      <formula2>11</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
center / 2023.02.14 / 21:35 / sojung
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/templates/template_센터.xlsx
+++ b/src/main/webapp/resources/templates/template_센터.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KOSA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KOSA\git\store-management\src\main\webapp\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7434E5BB-A45C-4F42-9EE8-2C7D61F2A704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE842E8-667C-435D-BE47-5A8AF08A6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4840" yWindow="1600" windowWidth="19200" windowHeight="11260" xr2:uid="{59DB4302-11B8-4813-85BF-B0C8E7845784}"/>
+    <workbookView xWindow="4070" yWindow="7320" windowWidth="19190" windowHeight="11260" xr2:uid="{59DB4302-11B8-4813-85BF-B0C8E7845784}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,12 +67,12 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t>수정 시 기존에 등록되어 있던 센터코드는 건들지마세요</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>전화번호, 오픈일, 폐점일은 숫자만 입력해주세요</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정 시 기존에 등록되어 있던 센터코드를 일치시켜주세요</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
   <dimension ref="B2:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -717,12 +717,12 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.45">
       <c r="J6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.45">
       <c r="J7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.45">

</xml_diff>